<commit_message>
1. add data read from DB
</commit_message>
<xml_diff>
--- a/xlsxResult/sanhabyaccount.xlsx
+++ b/xlsxResult/sanhabyaccount.xlsx
@@ -402,6 +402,16 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Actual by Account - 속초 컨피네스 비치 호텔</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Create Date : 2023-01-05 18:06:11</v>
+      </c>
+    </row>
     <row r="5">
       <c r="A5" t="str">
         <v>No</v>

</xml_diff>